<commit_message>
updated aim 3 analyses
</commit_message>
<xml_diff>
--- a/District harmonization/District_Changes.xlsx
+++ b/District harmonization/District_Changes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcgill.sharepoint.com/sites/PROSPERED_Group/Shared Documents/General/CIHR RSBY India/data/Linking code and CSVs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcgill.sharepoint.com/sites/PROSPERED_Group/Shared Documents/General/CIHR RSBY India/data/Linking code and CSVs/District harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="762" documentId="8_{B95B0D2E-E9D4-8740-A922-149F5228A517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8AE84788-8246-9B43-853C-B88E4114EE09}"/>
+  <xr:revisionPtr revIDLastSave="764" documentId="8_{B95B0D2E-E9D4-8740-A922-149F5228A517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4412FA8-7C8B-DE43-93D8-5D252F9AF4DA}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{D1D00CCF-82AB-6D4D-9728-F84D718C5775}"/>
   </bookViews>
@@ -1456,8 +1456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{575372E9-62C3-4E49-80CB-916BD0797513}">
   <dimension ref="A1:D130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54:XFD59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4663,15 +4663,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009FE99232C2A610489C05CA2A95C6B0DC" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="99e3d855f4612a477f80c26c84225e60">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="748de206-7911-403a-93a2-ff3feb5ad88e" xmlns:ns3="d391a701-1e72-4a9c-8e27-32ae852ac85b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9d24ec2972380c9becf470258562e41c" ns2:_="" ns3:_="">
     <xsd:import namespace="748de206-7911-403a-93a2-ff3feb5ad88e"/>
@@ -4902,15 +4893,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FDE1080-05E2-40DC-AFCB-2FF0EFA9E9BF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA9CD780-B0BD-40BC-A1F0-B37A41579C99}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4927,4 +4919,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FDE1080-05E2-40DC-AFCB-2FF0EFA9E9BF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>